<commit_message>
Add a few more categories
</commit_message>
<xml_diff>
--- a/data/raw/ExtraCategoriesBacteria.xlsx
+++ b/data/raw/ExtraCategoriesBacteria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16908" uniqueCount="8516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17268" uniqueCount="8696">
   <si>
     <t>0-20 cm bulk soil, Duennwald forest (Picea abies, Pinus sylvestris, Carpinus betulus, Acer pseudoplatanus, Quercus robur - Ilex aquifolium, Sorbus aucuparia, Rubus idaeus, Rhamnus frangula, Pteridium aquilinum, Polygonatum multiflorum, Deschampsia cf. cespitosa - Scleropodium purum, Eurhynchium praelongum, Polytrichum cf. pilosum), poor loamy sand, pH 3,7-4,5, humus 4-6 %, C/N ratio 18-20</t>
   </si>
@@ -25567,6 +25567,546 @@
   </si>
   <si>
     <t>tidal flat of Naozhou Island</t>
+  </si>
+  <si>
+    <t>Anzali Lagoon</t>
+  </si>
+  <si>
+    <t>brackish water pond for prawn culture</t>
+  </si>
+  <si>
+    <t>saline ecosystem</t>
+  </si>
+  <si>
+    <t>water sample from petroleum reservoir production brine</t>
+  </si>
+  <si>
+    <t>bank of a river with highly saline water</t>
+  </si>
+  <si>
+    <t>Cooum River Traverses, 72M, surface water, pre-monsoon</t>
+  </si>
+  <si>
+    <t>fresh wastewater canal</t>
+  </si>
+  <si>
+    <t>Freshwater sample from a stone collected in the Ru de Balory river, Evry (France)</t>
+  </si>
+  <si>
+    <t>River Yamuna</t>
+  </si>
+  <si>
+    <t>Chennai Harbour Traverses, near sea shore, surface water, monsoon</t>
+  </si>
+  <si>
+    <t>chalky sediments from a freshwater lake</t>
+  </si>
+  <si>
+    <t>Lonar Lake soil sediment</t>
+  </si>
+  <si>
+    <t>soil sediment from alkaline crater lake Lonar</t>
+  </si>
+  <si>
+    <t>Cotton Glacier</t>
+  </si>
+  <si>
+    <t>hydrothermal alkaline chimney of Prony Bay, New-Caledonia</t>
+  </si>
+  <si>
+    <t>hypersaline coastal marsh</t>
+  </si>
+  <si>
+    <t>mangrove estuary</t>
+  </si>
+  <si>
+    <t>Marina Beach marine water sample</t>
+  </si>
+  <si>
+    <t>Marine coastal environment</t>
+  </si>
+  <si>
+    <t>Ria Formosa</t>
+  </si>
+  <si>
+    <t>shallow water off the coast</t>
+  </si>
+  <si>
+    <t>coastal surface sediment approximately 80 cm below sea level</t>
+  </si>
+  <si>
+    <t>Deep Biosphere Sample (DeepBIOS, IODP Expedition 316)</t>
+  </si>
+  <si>
+    <t>marine sediment sampled from UXO-contaminated site UXO-1</t>
+  </si>
+  <si>
+    <t>marine sediment-water interface Fe-oxidizing biofilm</t>
+  </si>
+  <si>
+    <t>marine sediment; water depth 13.5 m</t>
+  </si>
+  <si>
+    <t>site MidRef, marine sediment in UXO clear zone</t>
+  </si>
+  <si>
+    <t>site UXO-5, UXO-contaminated marine sediment</t>
+  </si>
+  <si>
+    <t>mud and sand from sea shore</t>
+  </si>
+  <si>
+    <t>3-day old biofilm on glass developed at HKUST pier, Port Shelter</t>
+  </si>
+  <si>
+    <t>5-day old natural biofilm on polystyrene petri dish developed at fish farm, Long Harbor</t>
+  </si>
+  <si>
+    <t>fish farming pond</t>
+  </si>
+  <si>
+    <t>fresh irrigated water present in crop fields</t>
+  </si>
+  <si>
+    <t>mesophilic saline spring</t>
+  </si>
+  <si>
+    <t>thermal water</t>
+  </si>
+  <si>
+    <t>water bloom</t>
+  </si>
+  <si>
+    <t>water from loach farming pond</t>
+  </si>
+  <si>
+    <t>activated sludge from Aalborg East wastewater treatment plant</t>
+  </si>
+  <si>
+    <t>activated sludge of a waste water treatment plant</t>
+  </si>
+  <si>
+    <t>Anaerobic digester from Casolino (Italy) domestic wastewater treatment plant</t>
+  </si>
+  <si>
+    <t>Anaerobic digester from Manheim (Germany) domestic wastewater treatment plant</t>
+  </si>
+  <si>
+    <t>biofilm from a nitritation-anammox moving bed biofilm reactor (MBBR)</t>
+  </si>
+  <si>
+    <t>biofilm in a non-chlorinated drinking water reservoir</t>
+  </si>
+  <si>
+    <t>bioreactor inoculated with oil field produced water</t>
+  </si>
+  <si>
+    <t>Cattle Manure Compost</t>
+  </si>
+  <si>
+    <t>dairy effluent</t>
+  </si>
+  <si>
+    <t>domestic sewage canal water</t>
+  </si>
+  <si>
+    <t>enrichment culture of sediment from an acidic stream draining an abandoned copper mine</t>
+  </si>
+  <si>
+    <t>pesticide plant sludge</t>
+  </si>
+  <si>
+    <t>reactor</t>
+  </si>
+  <si>
+    <t>rice mill wastewater</t>
+  </si>
+  <si>
+    <t>sludge from a semi-continuous 45-L methanogenic reactor inoculated with cow manure and fed household water at mesophilic temperature</t>
+  </si>
+  <si>
+    <t>sludge from the effluent treatment pond from Cunha Baixa Uranium mine</t>
+  </si>
+  <si>
+    <t>subsurface clay soil/pine wood shavings incubation</t>
+  </si>
+  <si>
+    <t>subsurface clay soil/pine wood shavings incubation water</t>
+  </si>
+  <si>
+    <t>Swine lagoon in Faouet region (France)</t>
+  </si>
+  <si>
+    <t>cottage cheese, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>dry fish</t>
+  </si>
+  <si>
+    <t>fermented soybean paste and meju</t>
+  </si>
+  <si>
+    <t>home-made cheese 1, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 11, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 13, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 14, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 15, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 2, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 4, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 5, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 6, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made cheese 7, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>home-made soft cheese, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>kombucha</t>
+  </si>
+  <si>
+    <t>meju (Korean traditional soybean product starter)</t>
+  </si>
+  <si>
+    <t>pepper sauce from fermenting Spanish pepper</t>
+  </si>
+  <si>
+    <t>Red Oncom, Indonesian fermented food</t>
+  </si>
+  <si>
+    <t>matsoni, Erevan, Armenia</t>
+  </si>
+  <si>
+    <t>mixed vegetable pickle</t>
+  </si>
+  <si>
+    <t>lambic brewery air</t>
+  </si>
+  <si>
+    <t>Blue colour, icon A, Samanod Church</t>
+  </si>
+  <si>
+    <t>sample PS: wall showing purple stains</t>
+  </si>
+  <si>
+    <t>showerhead biofilm</t>
+  </si>
+  <si>
+    <t>contaminated groundwater of a solvent recycling factory</t>
+  </si>
+  <si>
+    <t>Gaft chromite mine</t>
+  </si>
+  <si>
+    <t>hotel sewage</t>
+  </si>
+  <si>
+    <t>organic waste of dump site</t>
+  </si>
+  <si>
+    <t>petroleum hydro carbon contaminated soil</t>
+  </si>
+  <si>
+    <t>soil from bauxite mine</t>
+  </si>
+  <si>
+    <t>textile dye factory effluent</t>
+  </si>
+  <si>
+    <t>waste of zob-Ahan factory</t>
+  </si>
+  <si>
+    <t>weathered copper mine spoil</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Arabidopsis seeds</t>
+  </si>
+  <si>
+    <t>fruit tissue</t>
+  </si>
+  <si>
+    <t>pumpkin fruit</t>
+  </si>
+  <si>
+    <t>vegetable waste used for microbial fuel cell (MFC) technology</t>
+  </si>
+  <si>
+    <t>Cholla flower</t>
+  </si>
+  <si>
+    <t>Oppuntia flower</t>
+  </si>
+  <si>
+    <t>Aconitum plant soil rhizosphere</t>
+  </si>
+  <si>
+    <t>endosphere of rice root</t>
+  </si>
+  <si>
+    <t>endosphere of rice roots</t>
+  </si>
+  <si>
+    <t>grapevine root system</t>
+  </si>
+  <si>
+    <t>grapevine roots</t>
+  </si>
+  <si>
+    <t>Halophyte rhizosphere</t>
+  </si>
+  <si>
+    <t>Phyllite soil of Korean ginseng rhizosphere</t>
+  </si>
+  <si>
+    <t>Podophyllum plant soil rhizosphere</t>
+  </si>
+  <si>
+    <t>rhizospheric sample of Echinocactus platyacanthus</t>
+  </si>
+  <si>
+    <t>rhizospheric soil of Bruguiera gymnorhiza</t>
+  </si>
+  <si>
+    <t>rhizospheric soil of rice roots</t>
+  </si>
+  <si>
+    <t>Rhododendron rhizosphere soil</t>
+  </si>
+  <si>
+    <t>soybean rhizosphere soil</t>
+  </si>
+  <si>
+    <t>tomato plant soil rhizosphere</t>
+  </si>
+  <si>
+    <t>Withania somnifera rhizosphere soil</t>
+  </si>
+  <si>
+    <t>host root, leaf</t>
+  </si>
+  <si>
+    <t>host root, stem</t>
+  </si>
+  <si>
+    <t>host root, stem, leaf</t>
+  </si>
+  <si>
+    <t>host stem, leaf</t>
+  </si>
+  <si>
+    <t>chestnut Wageningen</t>
+  </si>
+  <si>
+    <t>cyclamen leaf</t>
+  </si>
+  <si>
+    <t>Lamium maculatum</t>
+  </si>
+  <si>
+    <t>tissue of Pinus thunbergii</t>
+  </si>
+  <si>
+    <t>aguricutural soil</t>
+  </si>
+  <si>
+    <t>rice paddy field marshy soil</t>
+  </si>
+  <si>
+    <t>soil around cow dung</t>
+  </si>
+  <si>
+    <t>turmeric filed soil sample</t>
+  </si>
+  <si>
+    <t>desert rocks and monuments</t>
+  </si>
+  <si>
+    <t>healthy plant soil</t>
+  </si>
+  <si>
+    <t>military soil</t>
+  </si>
+  <si>
+    <t>rhizome soil</t>
+  </si>
+  <si>
+    <t>Upland field Soil</t>
+  </si>
+  <si>
+    <t>mud sample from gas station</t>
+  </si>
+  <si>
+    <t>petrol filling station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nymphal tick </t>
+  </si>
+  <si>
+    <t>testis of migratory locust</t>
+  </si>
+  <si>
+    <t>unfed tick</t>
+  </si>
+  <si>
+    <t>ANG gland of Sepia officinalis</t>
+  </si>
+  <si>
+    <t>calcareous sponge host</t>
+  </si>
+  <si>
+    <t>Sepia officinalis</t>
+  </si>
+  <si>
+    <t>gorgonian</t>
+  </si>
+  <si>
+    <t>arthritic elbow</t>
+  </si>
+  <si>
+    <t>blood from laboratory mouse</t>
+  </si>
+  <si>
+    <t>calf 16 months, State farm Moskovskiy, Moscow</t>
+  </si>
+  <si>
+    <t>cataract induced eye</t>
+  </si>
+  <si>
+    <t>dead host</t>
+  </si>
+  <si>
+    <t>febrile patient</t>
+  </si>
+  <si>
+    <t>Feces of wild westernlowland gorilla</t>
+  </si>
+  <si>
+    <t>gastric juice</t>
+  </si>
+  <si>
+    <t>gill tissue of diseased Tor putitora</t>
+  </si>
+  <si>
+    <t>gill tissue of Oncorhynchus mykiss</t>
+  </si>
+  <si>
+    <t>gull bladder</t>
+  </si>
+  <si>
+    <t>guppy</t>
+  </si>
+  <si>
+    <t>healthy human anticubital fosa</t>
+  </si>
+  <si>
+    <t>heart valve from patient with infective endocarditis</t>
+  </si>
+  <si>
+    <t>infected chipmunk blood injected into a mouse, infected mouse blood put into culture medium and DNA extracted from spirochetes that grew out in the culture medium</t>
+  </si>
+  <si>
+    <t>infected human blood injected into a mouse, infected mouse blood put into culture medium and DNA extracted from spirochetes that grew out in the culture medium</t>
+  </si>
+  <si>
+    <t>infected Ornithodoros hermsi tick fed on mouse, infected mouse blood put into culture medium and DNA extracted from spirochetes that grew out in the culture medium</t>
+  </si>
+  <si>
+    <t>lesion within broken skin-horn junction of host hoof</t>
+  </si>
+  <si>
+    <t>liver tissue</t>
+  </si>
+  <si>
+    <t>lower intestine</t>
+  </si>
+  <si>
+    <t>lower intestine of Oncorhynchus mykiss</t>
+  </si>
+  <si>
+    <t>newborn, 1 day</t>
+  </si>
+  <si>
+    <t>newborn, 3 days (mother-23 years old)</t>
+  </si>
+  <si>
+    <t>newborn, 4 months old</t>
+  </si>
+  <si>
+    <t>newborn, 5 days (mother 33 years old)</t>
+  </si>
+  <si>
+    <t>oral cavity dental plaque</t>
+  </si>
+  <si>
+    <t>patient with peritonsillar abscess</t>
+  </si>
+  <si>
+    <t>penguin rookery</t>
+  </si>
+  <si>
+    <t>right axilla aspirate</t>
+  </si>
+  <si>
+    <t>rumen of cattle (breed: Nellore steers)</t>
+  </si>
+  <si>
+    <t>Sea turtle egg</t>
+  </si>
+  <si>
+    <t>semen from a bull with vesiculitis</t>
+  </si>
+  <si>
+    <t>semen from a healthy bull</t>
+  </si>
+  <si>
+    <t>soft tissue</t>
+  </si>
+  <si>
+    <t>swab from lower jaw</t>
+  </si>
+  <si>
+    <t>swab from mouth</t>
+  </si>
+  <si>
+    <t>swab from upper jaw</t>
+  </si>
+  <si>
+    <t>Swine fece</t>
+  </si>
+  <si>
+    <t>wound swab from an 18 year old female diagnosed with a pilonidal cyst without abscess</t>
+  </si>
+  <si>
+    <t>BAS</t>
+  </si>
+  <si>
+    <t>caecitis</t>
+  </si>
+  <si>
+    <t>prawns</t>
+  </si>
+  <si>
+    <t>pulmonary puncture</t>
   </si>
 </sst>
 </file>
@@ -25960,11 +26500,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8454"/>
+  <dimension ref="A1:C8634"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8418" workbookViewId="0">
-      <selection activeCell="A8454" sqref="A8454"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -93610,6 +94148,1446 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8455" spans="1:3">
+      <c r="A8455" t="s">
+        <v>463</v>
+      </c>
+      <c r="B8455" t="s">
+        <v>8516</v>
+      </c>
+    </row>
+    <row r="8456" spans="1:3">
+      <c r="A8456" t="s">
+        <v>463</v>
+      </c>
+      <c r="B8456" t="s">
+        <v>8517</v>
+      </c>
+    </row>
+    <row r="8457" spans="1:3">
+      <c r="A8457" t="s">
+        <v>463</v>
+      </c>
+      <c r="B8457" t="s">
+        <v>8518</v>
+      </c>
+    </row>
+    <row r="8458" spans="1:3">
+      <c r="A8458" t="s">
+        <v>463</v>
+      </c>
+      <c r="B8458" t="s">
+        <v>8519</v>
+      </c>
+    </row>
+    <row r="8459" spans="1:3">
+      <c r="A8459" t="s">
+        <v>2125</v>
+      </c>
+      <c r="B8459" t="s">
+        <v>8520</v>
+      </c>
+    </row>
+    <row r="8460" spans="1:3">
+      <c r="A8460" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8460" t="s">
+        <v>8521</v>
+      </c>
+    </row>
+    <row r="8461" spans="1:3">
+      <c r="A8461" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8461" t="s">
+        <v>8522</v>
+      </c>
+    </row>
+    <row r="8462" spans="1:3">
+      <c r="A8462" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8462" t="s">
+        <v>8523</v>
+      </c>
+    </row>
+    <row r="8463" spans="1:3">
+      <c r="A8463" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8463" t="s">
+        <v>8524</v>
+      </c>
+    </row>
+    <row r="8464" spans="1:3">
+      <c r="A8464" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8464" t="s">
+        <v>8525</v>
+      </c>
+    </row>
+    <row r="8465" spans="1:2">
+      <c r="A8465" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8465" t="s">
+        <v>8526</v>
+      </c>
+    </row>
+    <row r="8466" spans="1:2">
+      <c r="A8466" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8466" t="s">
+        <v>8527</v>
+      </c>
+    </row>
+    <row r="8467" spans="1:2">
+      <c r="A8467" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8467" t="s">
+        <v>8528</v>
+      </c>
+    </row>
+    <row r="8468" spans="1:2">
+      <c r="A8468" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8468" t="s">
+        <v>8529</v>
+      </c>
+    </row>
+    <row r="8469" spans="1:2">
+      <c r="A8469" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8469" t="s">
+        <v>8530</v>
+      </c>
+    </row>
+    <row r="8470" spans="1:2">
+      <c r="A8470" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8470" t="s">
+        <v>8531</v>
+      </c>
+    </row>
+    <row r="8471" spans="1:2">
+      <c r="A8471" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8471" t="s">
+        <v>8532</v>
+      </c>
+    </row>
+    <row r="8472" spans="1:2">
+      <c r="A8472" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8472" t="s">
+        <v>8533</v>
+      </c>
+    </row>
+    <row r="8473" spans="1:2">
+      <c r="A8473" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8473" t="s">
+        <v>8534</v>
+      </c>
+    </row>
+    <row r="8474" spans="1:2">
+      <c r="A8474" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8474" t="s">
+        <v>8535</v>
+      </c>
+    </row>
+    <row r="8475" spans="1:2">
+      <c r="A8475" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8475" t="s">
+        <v>8536</v>
+      </c>
+    </row>
+    <row r="8476" spans="1:2">
+      <c r="A8476" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8476" t="s">
+        <v>8537</v>
+      </c>
+    </row>
+    <row r="8477" spans="1:2">
+      <c r="A8477" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8477" t="s">
+        <v>8538</v>
+      </c>
+    </row>
+    <row r="8478" spans="1:2">
+      <c r="A8478" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8478" t="s">
+        <v>8539</v>
+      </c>
+    </row>
+    <row r="8479" spans="1:2">
+      <c r="A8479" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8479" t="s">
+        <v>8540</v>
+      </c>
+    </row>
+    <row r="8480" spans="1:2">
+      <c r="A8480" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8480" t="s">
+        <v>8541</v>
+      </c>
+    </row>
+    <row r="8481" spans="1:2">
+      <c r="A8481" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8481" t="s">
+        <v>8542</v>
+      </c>
+    </row>
+    <row r="8482" spans="1:2">
+      <c r="A8482" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8482" t="s">
+        <v>8543</v>
+      </c>
+    </row>
+    <row r="8483" spans="1:2">
+      <c r="A8483" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8483" t="s">
+        <v>8544</v>
+      </c>
+    </row>
+    <row r="8484" spans="1:2">
+      <c r="A8484" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8484" t="s">
+        <v>8545</v>
+      </c>
+    </row>
+    <row r="8485" spans="1:2">
+      <c r="A8485" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8485" t="s">
+        <v>8546</v>
+      </c>
+    </row>
+    <row r="8486" spans="1:2">
+      <c r="A8486" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8486" t="s">
+        <v>8547</v>
+      </c>
+    </row>
+    <row r="8487" spans="1:2">
+      <c r="A8487" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8487" t="s">
+        <v>8548</v>
+      </c>
+    </row>
+    <row r="8488" spans="1:2">
+      <c r="A8488" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8488" t="s">
+        <v>8549</v>
+      </c>
+    </row>
+    <row r="8489" spans="1:2">
+      <c r="A8489" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8489" t="s">
+        <v>8550</v>
+      </c>
+    </row>
+    <row r="8490" spans="1:2">
+      <c r="A8490" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8490" t="s">
+        <v>8551</v>
+      </c>
+    </row>
+    <row r="8491" spans="1:2">
+      <c r="A8491" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8491" t="s">
+        <v>8552</v>
+      </c>
+    </row>
+    <row r="8492" spans="1:2">
+      <c r="A8492" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8492" t="s">
+        <v>8553</v>
+      </c>
+    </row>
+    <row r="8493" spans="1:2">
+      <c r="A8493" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8493" t="s">
+        <v>8554</v>
+      </c>
+    </row>
+    <row r="8494" spans="1:2">
+      <c r="A8494" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8494" t="s">
+        <v>8555</v>
+      </c>
+    </row>
+    <row r="8495" spans="1:2">
+      <c r="A8495" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8495" t="s">
+        <v>8556</v>
+      </c>
+    </row>
+    <row r="8496" spans="1:2">
+      <c r="A8496" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8496" t="s">
+        <v>8557</v>
+      </c>
+    </row>
+    <row r="8497" spans="1:2">
+      <c r="A8497" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8497" t="s">
+        <v>8558</v>
+      </c>
+    </row>
+    <row r="8498" spans="1:2">
+      <c r="A8498" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8498" t="s">
+        <v>8559</v>
+      </c>
+    </row>
+    <row r="8499" spans="1:2">
+      <c r="A8499" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8499" t="s">
+        <v>8560</v>
+      </c>
+    </row>
+    <row r="8500" spans="1:2">
+      <c r="A8500" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8500" t="s">
+        <v>8561</v>
+      </c>
+    </row>
+    <row r="8501" spans="1:2">
+      <c r="A8501" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8501" t="s">
+        <v>8562</v>
+      </c>
+    </row>
+    <row r="8502" spans="1:2">
+      <c r="A8502" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8502" t="s">
+        <v>8563</v>
+      </c>
+    </row>
+    <row r="8503" spans="1:2">
+      <c r="A8503" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8503" t="s">
+        <v>8564</v>
+      </c>
+    </row>
+    <row r="8504" spans="1:2">
+      <c r="A8504" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8504" t="s">
+        <v>8565</v>
+      </c>
+    </row>
+    <row r="8505" spans="1:2">
+      <c r="A8505" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8505" t="s">
+        <v>8566</v>
+      </c>
+    </row>
+    <row r="8506" spans="1:2">
+      <c r="A8506" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8506" t="s">
+        <v>8567</v>
+      </c>
+    </row>
+    <row r="8507" spans="1:2">
+      <c r="A8507" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8507" t="s">
+        <v>8568</v>
+      </c>
+    </row>
+    <row r="8508" spans="1:2">
+      <c r="A8508" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8508" t="s">
+        <v>8569</v>
+      </c>
+    </row>
+    <row r="8509" spans="1:2">
+      <c r="A8509" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8509" t="s">
+        <v>8570</v>
+      </c>
+    </row>
+    <row r="8510" spans="1:2">
+      <c r="A8510" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8510" t="s">
+        <v>8571</v>
+      </c>
+    </row>
+    <row r="8511" spans="1:2">
+      <c r="A8511" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8511" t="s">
+        <v>8572</v>
+      </c>
+    </row>
+    <row r="8512" spans="1:2">
+      <c r="A8512" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8512" t="s">
+        <v>8573</v>
+      </c>
+    </row>
+    <row r="8513" spans="1:2">
+      <c r="A8513" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8513" t="s">
+        <v>8574</v>
+      </c>
+    </row>
+    <row r="8514" spans="1:2">
+      <c r="A8514" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8514" t="s">
+        <v>8575</v>
+      </c>
+    </row>
+    <row r="8515" spans="1:2">
+      <c r="A8515" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8515" t="s">
+        <v>8576</v>
+      </c>
+    </row>
+    <row r="8516" spans="1:2">
+      <c r="A8516" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8516" t="s">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="8517" spans="1:2">
+      <c r="A8517" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8517" t="s">
+        <v>8578</v>
+      </c>
+    </row>
+    <row r="8518" spans="1:2">
+      <c r="A8518" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8518" t="s">
+        <v>8579</v>
+      </c>
+    </row>
+    <row r="8519" spans="1:2">
+      <c r="A8519" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8519" t="s">
+        <v>8580</v>
+      </c>
+    </row>
+    <row r="8520" spans="1:2">
+      <c r="A8520" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8520" t="s">
+        <v>8581</v>
+      </c>
+    </row>
+    <row r="8521" spans="1:2">
+      <c r="A8521" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8521" t="s">
+        <v>8582</v>
+      </c>
+    </row>
+    <row r="8522" spans="1:2">
+      <c r="A8522" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8522" t="s">
+        <v>8583</v>
+      </c>
+    </row>
+    <row r="8523" spans="1:2">
+      <c r="A8523" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8523" t="s">
+        <v>8584</v>
+      </c>
+    </row>
+    <row r="8524" spans="1:2">
+      <c r="A8524" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8524" t="s">
+        <v>8585</v>
+      </c>
+    </row>
+    <row r="8525" spans="1:2">
+      <c r="A8525" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8525" t="s">
+        <v>8586</v>
+      </c>
+    </row>
+    <row r="8526" spans="1:2">
+      <c r="A8526" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8526" t="s">
+        <v>8587</v>
+      </c>
+    </row>
+    <row r="8527" spans="1:2">
+      <c r="A8527" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8527" t="s">
+        <v>8588</v>
+      </c>
+    </row>
+    <row r="8528" spans="1:2">
+      <c r="A8528" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8528" t="s">
+        <v>8589</v>
+      </c>
+    </row>
+    <row r="8529" spans="1:2">
+      <c r="A8529" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8529" t="s">
+        <v>8590</v>
+      </c>
+    </row>
+    <row r="8530" spans="1:2">
+      <c r="A8530" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8530" t="s">
+        <v>8591</v>
+      </c>
+    </row>
+    <row r="8531" spans="1:2">
+      <c r="A8531" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B8531" t="s">
+        <v>8592</v>
+      </c>
+    </row>
+    <row r="8532" spans="1:2">
+      <c r="A8532" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B8532" t="s">
+        <v>8593</v>
+      </c>
+    </row>
+    <row r="8533" spans="1:2">
+      <c r="A8533" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B8533" t="s">
+        <v>8594</v>
+      </c>
+    </row>
+    <row r="8534" spans="1:2">
+      <c r="A8534" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B8534" t="s">
+        <v>8595</v>
+      </c>
+    </row>
+    <row r="8535" spans="1:2">
+      <c r="A8535" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8535" t="s">
+        <v>8596</v>
+      </c>
+    </row>
+    <row r="8536" spans="1:2">
+      <c r="A8536" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8536" t="s">
+        <v>8597</v>
+      </c>
+    </row>
+    <row r="8537" spans="1:2">
+      <c r="A8537" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8537" t="s">
+        <v>8598</v>
+      </c>
+    </row>
+    <row r="8538" spans="1:2">
+      <c r="A8538" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8538" t="s">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="8539" spans="1:2">
+      <c r="A8539" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8539" t="s">
+        <v>8600</v>
+      </c>
+    </row>
+    <row r="8540" spans="1:2">
+      <c r="A8540" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8540" t="s">
+        <v>8601</v>
+      </c>
+    </row>
+    <row r="8541" spans="1:2">
+      <c r="A8541" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8541" t="s">
+        <v>8602</v>
+      </c>
+    </row>
+    <row r="8542" spans="1:2">
+      <c r="A8542" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8542" t="s">
+        <v>8603</v>
+      </c>
+    </row>
+    <row r="8543" spans="1:2">
+      <c r="A8543" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8543" t="s">
+        <v>8604</v>
+      </c>
+    </row>
+    <row r="8544" spans="1:2">
+      <c r="A8544" t="s">
+        <v>3539</v>
+      </c>
+      <c r="B8544" t="s">
+        <v>8605</v>
+      </c>
+    </row>
+    <row r="8545" spans="1:2">
+      <c r="A8545" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8545" t="s">
+        <v>8606</v>
+      </c>
+    </row>
+    <row r="8546" spans="1:2">
+      <c r="A8546" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8546" t="s">
+        <v>8607</v>
+      </c>
+    </row>
+    <row r="8547" spans="1:2">
+      <c r="A8547" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8547" t="s">
+        <v>8608</v>
+      </c>
+    </row>
+    <row r="8548" spans="1:2">
+      <c r="A8548" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8548" t="s">
+        <v>8609</v>
+      </c>
+    </row>
+    <row r="8549" spans="1:2">
+      <c r="A8549" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8549" t="s">
+        <v>8610</v>
+      </c>
+    </row>
+    <row r="8550" spans="1:2">
+      <c r="A8550" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8550" t="s">
+        <v>8611</v>
+      </c>
+    </row>
+    <row r="8551" spans="1:2">
+      <c r="A8551" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8551" t="s">
+        <v>8612</v>
+      </c>
+    </row>
+    <row r="8552" spans="1:2">
+      <c r="A8552" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8552" t="s">
+        <v>8613</v>
+      </c>
+    </row>
+    <row r="8553" spans="1:2">
+      <c r="A8553" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8553" t="s">
+        <v>8614</v>
+      </c>
+    </row>
+    <row r="8554" spans="1:2">
+      <c r="A8554" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8554" t="s">
+        <v>8615</v>
+      </c>
+    </row>
+    <row r="8555" spans="1:2">
+      <c r="A8555" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8555" t="s">
+        <v>8616</v>
+      </c>
+    </row>
+    <row r="8556" spans="1:2">
+      <c r="A8556" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8556" t="s">
+        <v>8617</v>
+      </c>
+    </row>
+    <row r="8557" spans="1:2">
+      <c r="A8557" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8557" t="s">
+        <v>8618</v>
+      </c>
+    </row>
+    <row r="8558" spans="1:2">
+      <c r="A8558" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8558" t="s">
+        <v>8619</v>
+      </c>
+    </row>
+    <row r="8559" spans="1:2">
+      <c r="A8559" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8559" t="s">
+        <v>8620</v>
+      </c>
+    </row>
+    <row r="8560" spans="1:2">
+      <c r="A8560" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8560" t="s">
+        <v>8621</v>
+      </c>
+    </row>
+    <row r="8561" spans="1:2">
+      <c r="A8561" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8561" t="s">
+        <v>8622</v>
+      </c>
+    </row>
+    <row r="8562" spans="1:2">
+      <c r="A8562" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8562" t="s">
+        <v>8623</v>
+      </c>
+    </row>
+    <row r="8563" spans="1:2">
+      <c r="A8563" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8563" t="s">
+        <v>8624</v>
+      </c>
+    </row>
+    <row r="8564" spans="1:2">
+      <c r="A8564" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8564" t="s">
+        <v>8625</v>
+      </c>
+    </row>
+    <row r="8565" spans="1:2">
+      <c r="A8565" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8565" t="s">
+        <v>8626</v>
+      </c>
+    </row>
+    <row r="8566" spans="1:2">
+      <c r="A8566" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8566" t="s">
+        <v>8627</v>
+      </c>
+    </row>
+    <row r="8567" spans="1:2">
+      <c r="A8567" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8567" t="s">
+        <v>8628</v>
+      </c>
+    </row>
+    <row r="8568" spans="1:2">
+      <c r="A8568" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8568" t="s">
+        <v>8629</v>
+      </c>
+    </row>
+    <row r="8569" spans="1:2">
+      <c r="A8569" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8569" t="s">
+        <v>8630</v>
+      </c>
+    </row>
+    <row r="8570" spans="1:2">
+      <c r="A8570" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8570" t="s">
+        <v>8631</v>
+      </c>
+    </row>
+    <row r="8571" spans="1:2">
+      <c r="A8571" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8571" t="s">
+        <v>8632</v>
+      </c>
+    </row>
+    <row r="8572" spans="1:2">
+      <c r="A8572" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8572" t="s">
+        <v>8633</v>
+      </c>
+    </row>
+    <row r="8573" spans="1:2">
+      <c r="A8573" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8573" t="s">
+        <v>8634</v>
+      </c>
+    </row>
+    <row r="8574" spans="1:2">
+      <c r="A8574" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8574" t="s">
+        <v>8635</v>
+      </c>
+    </row>
+    <row r="8575" spans="1:2">
+      <c r="A8575" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8575" t="s">
+        <v>8636</v>
+      </c>
+    </row>
+    <row r="8576" spans="1:2">
+      <c r="A8576" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8576" t="s">
+        <v>8637</v>
+      </c>
+    </row>
+    <row r="8577" spans="1:2">
+      <c r="A8577" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8577" t="s">
+        <v>8638</v>
+      </c>
+    </row>
+    <row r="8578" spans="1:2">
+      <c r="A8578" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8578" t="s">
+        <v>8639</v>
+      </c>
+    </row>
+    <row r="8579" spans="1:2">
+      <c r="A8579" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8579" t="s">
+        <v>8640</v>
+      </c>
+    </row>
+    <row r="8580" spans="1:2">
+      <c r="A8580" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8580" t="s">
+        <v>8641</v>
+      </c>
+    </row>
+    <row r="8581" spans="1:2">
+      <c r="A8581" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8581" t="s">
+        <v>8642</v>
+      </c>
+    </row>
+    <row r="8582" spans="1:2">
+      <c r="A8582" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8582" t="s">
+        <v>8643</v>
+      </c>
+    </row>
+    <row r="8583" spans="1:2">
+      <c r="A8583" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8583" t="s">
+        <v>8644</v>
+      </c>
+    </row>
+    <row r="8584" spans="1:2">
+      <c r="A8584" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8584" t="s">
+        <v>8645</v>
+      </c>
+    </row>
+    <row r="8585" spans="1:2">
+      <c r="A8585" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8585" t="s">
+        <v>8646</v>
+      </c>
+    </row>
+    <row r="8586" spans="1:2">
+      <c r="A8586" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8586" t="s">
+        <v>8647</v>
+      </c>
+    </row>
+    <row r="8587" spans="1:2">
+      <c r="A8587" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8587" t="s">
+        <v>8648</v>
+      </c>
+    </row>
+    <row r="8588" spans="1:2">
+      <c r="A8588" t="s">
+        <v>3616</v>
+      </c>
+      <c r="B8588" t="s">
+        <v>8649</v>
+      </c>
+    </row>
+    <row r="8589" spans="1:2">
+      <c r="A8589" t="s">
+        <v>3616</v>
+      </c>
+      <c r="B8589" t="s">
+        <v>8650</v>
+      </c>
+    </row>
+    <row r="8590" spans="1:2">
+      <c r="A8590" t="s">
+        <v>3616</v>
+      </c>
+      <c r="B8590" t="s">
+        <v>8651</v>
+      </c>
+    </row>
+    <row r="8591" spans="1:2">
+      <c r="A8591" t="s">
+        <v>3616</v>
+      </c>
+      <c r="B8591" t="s">
+        <v>8652</v>
+      </c>
+    </row>
+    <row r="8592" spans="1:2">
+      <c r="A8592" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8592" t="s">
+        <v>8653</v>
+      </c>
+    </row>
+    <row r="8593" spans="1:2">
+      <c r="A8593" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8593" t="s">
+        <v>8654</v>
+      </c>
+    </row>
+    <row r="8594" spans="1:2">
+      <c r="A8594" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8594" t="s">
+        <v>8655</v>
+      </c>
+    </row>
+    <row r="8595" spans="1:2">
+      <c r="A8595" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8595" t="s">
+        <v>8656</v>
+      </c>
+    </row>
+    <row r="8596" spans="1:2">
+      <c r="A8596" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8596" t="s">
+        <v>8657</v>
+      </c>
+    </row>
+    <row r="8597" spans="1:2">
+      <c r="A8597" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8597" t="s">
+        <v>8658</v>
+      </c>
+    </row>
+    <row r="8598" spans="1:2">
+      <c r="A8598" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8598" t="s">
+        <v>8659</v>
+      </c>
+    </row>
+    <row r="8599" spans="1:2">
+      <c r="A8599" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8599" t="s">
+        <v>8660</v>
+      </c>
+    </row>
+    <row r="8600" spans="1:2">
+      <c r="A8600" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8600" t="s">
+        <v>8661</v>
+      </c>
+    </row>
+    <row r="8601" spans="1:2">
+      <c r="A8601" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8601" t="s">
+        <v>8662</v>
+      </c>
+    </row>
+    <row r="8602" spans="1:2">
+      <c r="A8602" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8602" t="s">
+        <v>8663</v>
+      </c>
+    </row>
+    <row r="8603" spans="1:2">
+      <c r="A8603" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8603" t="s">
+        <v>8664</v>
+      </c>
+    </row>
+    <row r="8604" spans="1:2">
+      <c r="A8604" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8604" t="s">
+        <v>8665</v>
+      </c>
+    </row>
+    <row r="8605" spans="1:2">
+      <c r="A8605" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8605" t="s">
+        <v>8666</v>
+      </c>
+    </row>
+    <row r="8606" spans="1:2">
+      <c r="A8606" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8606" t="s">
+        <v>8667</v>
+      </c>
+    </row>
+    <row r="8607" spans="1:2">
+      <c r="A8607" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8607" t="s">
+        <v>8668</v>
+      </c>
+    </row>
+    <row r="8608" spans="1:2">
+      <c r="A8608" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8608" t="s">
+        <v>8669</v>
+      </c>
+    </row>
+    <row r="8609" spans="1:2">
+      <c r="A8609" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8609" t="s">
+        <v>8670</v>
+      </c>
+    </row>
+    <row r="8610" spans="1:2">
+      <c r="A8610" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8610" t="s">
+        <v>8671</v>
+      </c>
+    </row>
+    <row r="8611" spans="1:2">
+      <c r="A8611" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8611" t="s">
+        <v>8672</v>
+      </c>
+    </row>
+    <row r="8612" spans="1:2">
+      <c r="A8612" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8612" t="s">
+        <v>8673</v>
+      </c>
+    </row>
+    <row r="8613" spans="1:2">
+      <c r="A8613" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8613" t="s">
+        <v>8674</v>
+      </c>
+    </row>
+    <row r="8614" spans="1:2">
+      <c r="A8614" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8614" t="s">
+        <v>8675</v>
+      </c>
+    </row>
+    <row r="8615" spans="1:2">
+      <c r="A8615" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8615" t="s">
+        <v>8676</v>
+      </c>
+    </row>
+    <row r="8616" spans="1:2">
+      <c r="A8616" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8616" t="s">
+        <v>8677</v>
+      </c>
+    </row>
+    <row r="8617" spans="1:2">
+      <c r="A8617" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8617" t="s">
+        <v>8678</v>
+      </c>
+    </row>
+    <row r="8618" spans="1:2">
+      <c r="A8618" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8618" t="s">
+        <v>8679</v>
+      </c>
+    </row>
+    <row r="8619" spans="1:2">
+      <c r="A8619" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8619" t="s">
+        <v>8680</v>
+      </c>
+    </row>
+    <row r="8620" spans="1:2">
+      <c r="A8620" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8620" t="s">
+        <v>8681</v>
+      </c>
+    </row>
+    <row r="8621" spans="1:2">
+      <c r="A8621" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8621" t="s">
+        <v>8682</v>
+      </c>
+    </row>
+    <row r="8622" spans="1:2">
+      <c r="A8622" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8622" t="s">
+        <v>8683</v>
+      </c>
+    </row>
+    <row r="8623" spans="1:2">
+      <c r="A8623" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8623" t="s">
+        <v>8684</v>
+      </c>
+    </row>
+    <row r="8624" spans="1:2">
+      <c r="A8624" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8624" t="s">
+        <v>8685</v>
+      </c>
+    </row>
+    <row r="8625" spans="1:2">
+      <c r="A8625" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8625" t="s">
+        <v>8686</v>
+      </c>
+    </row>
+    <row r="8626" spans="1:2">
+      <c r="A8626" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8626" t="s">
+        <v>8687</v>
+      </c>
+    </row>
+    <row r="8627" spans="1:2">
+      <c r="A8627" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8627" t="s">
+        <v>8688</v>
+      </c>
+    </row>
+    <row r="8628" spans="1:2">
+      <c r="A8628" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8628" t="s">
+        <v>8689</v>
+      </c>
+    </row>
+    <row r="8629" spans="1:2">
+      <c r="A8629" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8629" t="s">
+        <v>8690</v>
+      </c>
+    </row>
+    <row r="8630" spans="1:2">
+      <c r="A8630" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8630" t="s">
+        <v>8691</v>
+      </c>
+    </row>
+    <row r="8631" spans="1:2">
+      <c r="A8631" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8631" t="s">
+        <v>8692</v>
+      </c>
+    </row>
+    <row r="8632" spans="1:2">
+      <c r="A8632" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8632" t="s">
+        <v>8693</v>
+      </c>
+    </row>
+    <row r="8633" spans="1:2">
+      <c r="A8633" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8633" t="s">
+        <v>8694</v>
+      </c>
+    </row>
+    <row r="8634" spans="1:2">
+      <c r="A8634" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8634" t="s">
+        <v>8695</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>